<commit_message>
Correct benchmark table file
</commit_message>
<xml_diff>
--- a/dz/03_benchmark/benchmark_table.xlsx
+++ b/dz/03_benchmark/benchmark_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgijmamarin/Desktop/Figaro_bot/Figaro_bot-2/Figaro/dz/03_benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDA7419F-E79D-C94A-BFC8-6326D9BD6120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708A0CEE-A6B8-C74A-A278-A01CC5FB2CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11140" yWindow="-25740" windowWidth="30620" windowHeight="15740" xr2:uid="{F857EE3F-9DD7-8043-8427-5C7423A82846}"/>
   </bookViews>
@@ -1228,7 +1228,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>